<commit_message>
Autoreferencia a archivo de mineria
Se agregó, en los metadatos del indicador, referencia hacia el archivo de minería en el repositorio de Github.
</commit_message>
<xml_diff>
--- a/AG0102_Viviendas que cuentan con agua entubada.xlsx
+++ b/AG0102_Viviendas que cuentan con agua entubada.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="7665" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="7665"/>
   </bookViews>
   <sheets>
     <sheet name="METADATOS" sheetId="5" r:id="rId1"/>
@@ -25,14 +25,14 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
-    <pivotCache cacheId="1" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId6"/>
+    <pivotCache cacheId="4" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5654" uniqueCount="2052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5657" uniqueCount="2054">
   <si>
     <t>NOM_ENT</t>
   </si>
@@ -6198,6 +6198,12 @@
     <t>Revisión de existencia de la información en el Dataset disponible
 TRUE = El Municipio cuenta con información en el dataset
 FALSE = El Municipio no cuenta con información en el dataset</t>
+  </si>
+  <si>
+    <t>https://github.com/Caranarq/AG0102/blob/master/AG0102.py</t>
+  </si>
+  <si>
+    <t>Archivo de minería</t>
   </si>
 </sst>
 </file>
@@ -6207,7 +6213,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6262,6 +6268,14 @@
       <color theme="1"/>
       <name val="Soberana Sans"/>
       <family val="3"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -6348,11 +6362,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -6405,9 +6420,13 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -14911,7 +14930,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
   <location ref="J1:K51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" subtotalTop="0" showAll="0">
@@ -15150,7 +15169,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="J3:K7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -15580,10 +15599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15782,13 +15801,32 @@
         <v>2008</v>
       </c>
     </row>
+    <row r="26" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:2" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="22" t="s">
+        <v>1983</v>
+      </c>
+      <c r="B27" s="22"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>2053</v>
+      </c>
+      <c r="B28" s="24" t="s">
+        <v>2052</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B28" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -15796,7 +15834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Correccion a informacion de metadatos
Correccion metadatos
</commit_message>
<xml_diff>
--- a/AG0102_Viviendas que cuentan con agua entubada.xlsx
+++ b/AG0102_Viviendas que cuentan con agua entubada.xlsx
@@ -25,14 +25,14 @@
   </definedNames>
   <calcPr calcId="171027"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId6"/>
-    <pivotCache cacheId="4" r:id="rId7"/>
+    <pivotCache cacheId="5" r:id="rId6"/>
+    <pivotCache cacheId="6" r:id="rId7"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5657" uniqueCount="2054">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5657" uniqueCount="2055">
   <si>
     <t>NOM_ENT</t>
   </si>
@@ -6203,7 +6203,10 @@
     <t>https://github.com/Caranarq/AG0102/blob/master/AG0102.py</t>
   </si>
   <si>
-    <t>Archivo de minería</t>
+    <t>Archivo de minería de datos</t>
+  </si>
+  <si>
+    <t>Scripts</t>
   </si>
 </sst>
 </file>
@@ -6414,14 +6417,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -14930,7 +14933,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8" fieldListSortAscending="1">
   <location ref="J1:K51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" subtotalTop="0" showAll="0">
@@ -15169,7 +15172,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="10">
   <location ref="J3:K7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" subtotalTop="0" showAll="0"/>
@@ -15602,7 +15605,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -15629,10 +15632,10 @@
     </row>
     <row r="2" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:9" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="23" t="s">
         <v>1973</v>
       </c>
-      <c r="B3" s="22"/>
+      <c r="B3" s="23"/>
     </row>
     <row r="4" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
@@ -15676,10 +15679,10 @@
     </row>
     <row r="9" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:9" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="23" t="s">
         <v>1983</v>
       </c>
-      <c r="B10" s="22"/>
+      <c r="B10" s="23"/>
     </row>
     <row r="11" spans="1:9" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
@@ -15803,16 +15806,16 @@
     </row>
     <row r="26" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:2" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="22" t="s">
-        <v>1983</v>
-      </c>
-      <c r="B27" s="22"/>
+      <c r="A27" s="23" t="s">
+        <v>2053</v>
+      </c>
+      <c r="B27" s="23"/>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>2053</v>
-      </c>
-      <c r="B28" s="24" t="s">
+        <v>2054</v>
+      </c>
+      <c r="B28" s="22" t="s">
         <v>2052</v>
       </c>
     </row>
@@ -15851,16 +15854,16 @@
       <c r="A1" s="19" t="s">
         <v>1972</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="24" t="s">
         <v>2050</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">

</xml_diff>

<commit_message>
Aclaraciones a fuentes de información
Aclaraciones a fuentes de informacion para scripts locales (SUN y SUN_Integridad)
</commit_message>
<xml_diff>
--- a/AG0102_Viviendas que cuentan con agua entubada.xlsx
+++ b/AG0102_Viviendas que cuentan con agua entubada.xlsx
@@ -15607,7 +15607,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15839,7 +15841,7 @@
   <dimension ref="A1:L56"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -16355,7 +16357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O295"/>
   <sheetViews>
-    <sheetView topLeftCell="C109" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="E291" sqref="E291"/>
     </sheetView>
   </sheetViews>

</xml_diff>